<commit_message>
jsonjsdb_editor - added : name and parent_ids to history entries of type delete
</commit_message>
<xml_diff>
--- a/jsonjsdb_editor/test/excel_version/basic/db/tag.xlsx
+++ b/jsonjsdb_editor/test/excel_version/basic/db/tag.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb_editor/test/excel_version/db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb/jsonjsdb_editor/test/excel_version/basic/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8ADACD-A8AD-1A46-BC0C-92B4FEBEE3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFFFBD1-B941-9B41-8C0D-AE5FFB51A1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>tag_3</t>
+  </si>
+  <si>
+    <t>parent_id</t>
   </si>
 </sst>
 </file>
@@ -416,23 +419,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -440,20 +446,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jsonjsdb_editor - changed : replace column parent_ids by parent_entity_id by getting only the first column with suffix "_id"
</commit_message>
<xml_diff>
--- a/jsonjsdb_editor/test/excel_version/basic/db/tag.xlsx
+++ b/jsonjsdb_editor/test/excel_version/basic/db/tag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb/jsonjsdb_editor/test/excel_version/basic/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFFFBD1-B941-9B41-8C0D-AE5FFB51A1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAF8FBD-5838-D347-871F-5398F03C14BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -49,10 +49,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -422,7 +428,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,8 +459,8 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="C3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -464,11 +470,12 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
jsonjsdb_editor : changed : make jsonjsdb_editor use xlsx state for history so we can edit it manually
</commit_message>
<xml_diff>
--- a/jsonjsdb_editor/test/excel_version/basic/db/tag.xlsx
+++ b/jsonjsdb_editor/test/excel_version/basic/db/tag.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/mylib/jsonjsdb/jsonjsdb_editor/test/excel_version/basic/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAF8FBD-5838-D347-871F-5398F03C14BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B552ADB-148D-3141-BF14-6910D4DEEF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,10 +39,10 @@
     <t>tag_2</t>
   </si>
   <si>
-    <t>tag_3</t>
-  </si>
-  <si>
     <t>parent_id</t>
+  </si>
+  <si>
+    <t>tag_333</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,7 +441,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -468,7 +468,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>2</v>

</xml_diff>